<commit_message>
doc(add): continued info.md added content plus code description
</commit_message>
<xml_diff>
--- a/Dokumente/Planen/Projektablauf_Gantt.xlsx
+++ b/Dokumente/Planen/Projektablauf_Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/yves_jaros_edu_gbssg_ch/Documents/000_Schule_IMS-T1a/000_IMS/001-IntegriertePraxisarbeit/2025_TerminalChat/Dokumente/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/yves_jaros_edu_gbssg_ch/Documents/000_Schule_IMS-T1a/000_IMS/001-IntegriertePraxisarbeit/2025_TerminalChat/Dokumente/Planen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D7E4EBFE-A1CD-4CA4-901D-6FF22ED8BFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC1F04E-2C9F-4470-979B-30A8E973D01A}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{D7E4EBFE-A1CD-4CA4-901D-6FF22ED8BFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C34A6E9-E016-40CD-B22D-A6023E347A23}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="101">
   <si>
     <t>IPERKA</t>
   </si>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t>Kriegt jeder nutzer eine ID oder hängt die identifikation mit der IP-Adresse zusammen?</t>
+  </si>
+  <si>
+    <t>Code beispiel</t>
+  </si>
+  <si>
+    <t>Codebeispiel finden/ generieren</t>
+  </si>
+  <si>
+    <t>Codebeispiel ausprobieren testen</t>
+  </si>
+  <si>
+    <t>Codebeispiel verstehen</t>
   </si>
 </sst>
 </file>
@@ -349,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +383,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -801,6 +825,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1086,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ46"/>
+  <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT20" sqref="AT20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,9 +1135,10 @@
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="53" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1295,25 +1333,25 @@
       <c r="AA2" s="20"/>
       <c r="AB2" s="20"/>
       <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
+      <c r="AD2" s="47"/>
       <c r="AE2" s="20"/>
       <c r="AF2" s="20"/>
       <c r="AG2" s="20"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
+      <c r="AJ2" s="47"/>
       <c r="AK2" s="20"/>
       <c r="AL2" s="20"/>
       <c r="AM2" s="20"/>
       <c r="AN2" s="20"/>
       <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
+      <c r="AP2" s="47"/>
       <c r="AQ2" s="20"/>
       <c r="AR2" s="20"/>
       <c r="AS2" s="20"/>
       <c r="AT2" s="20"/>
       <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
+      <c r="AV2" s="47"/>
       <c r="AW2" s="20"/>
       <c r="AX2" s="20"/>
       <c r="AY2" s="20"/>
@@ -1339,9 +1377,9 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="45"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="P3" s="45"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -1355,25 +1393,25 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="AD3" s="48"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
+      <c r="AJ3" s="48"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
+      <c r="AP3" s="48"/>
       <c r="AQ3" s="2"/>
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
       <c r="AT3" s="2"/>
       <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
+      <c r="AV3" s="48"/>
       <c r="AW3" s="2"/>
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
@@ -1399,7 +1437,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="P4" s="45"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -1413,25 +1451,25 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
+      <c r="AD4" s="48"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
+      <c r="AJ4" s="48"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
+      <c r="AP4" s="48"/>
       <c r="AQ4" s="2"/>
       <c r="AR4" s="2"/>
       <c r="AS4" s="2"/>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
-      <c r="AV4" s="2"/>
+      <c r="AV4" s="48"/>
       <c r="AW4" s="2"/>
       <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
@@ -1457,7 +1495,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="P5" s="45"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -1471,25 +1509,25 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
+      <c r="AD5" s="48"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
+      <c r="AJ5" s="48"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
-      <c r="AP5" s="2"/>
+      <c r="AP5" s="48"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
-      <c r="AV5" s="2"/>
+      <c r="AV5" s="48"/>
       <c r="AW5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
@@ -1515,7 +1553,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="P6" s="45"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -1529,25 +1567,25 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
+      <c r="AD6" s="48"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
+      <c r="AJ6" s="48"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
+      <c r="AP6" s="48"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
-      <c r="AV6" s="2"/>
+      <c r="AV6" s="48"/>
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
@@ -1587,25 +1625,25 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
+      <c r="AD7" s="48"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
+      <c r="AJ7" s="48"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
+      <c r="AP7" s="48"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
-      <c r="AV7" s="2"/>
+      <c r="AV7" s="48"/>
       <c r="AW7" s="2"/>
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
@@ -1647,25 +1685,25 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
+      <c r="AD8" s="48"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
+      <c r="AJ8" s="48"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
+      <c r="AP8" s="48"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
-      <c r="AV8" s="2"/>
+      <c r="AV8" s="48"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
@@ -1705,25 +1743,25 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
+      <c r="AD9" s="48"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
+      <c r="AJ9" s="48"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
+      <c r="AP9" s="48"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
       <c r="AS9" s="2"/>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
-      <c r="AV9" s="2"/>
+      <c r="AV9" s="48"/>
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
@@ -1763,25 +1801,25 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
+      <c r="AD10" s="48"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-      <c r="AJ10" s="2"/>
+      <c r="AJ10" s="48"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
-      <c r="AP10" s="2"/>
+      <c r="AP10" s="48"/>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2"/>
       <c r="AS10" s="2"/>
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
-      <c r="AV10" s="2"/>
+      <c r="AV10" s="48"/>
       <c r="AW10" s="2"/>
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
@@ -1821,25 +1859,25 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
+      <c r="AD11" s="48"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
+      <c r="AJ11" s="48"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
-      <c r="AP11" s="2"/>
+      <c r="AP11" s="48"/>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
       <c r="AS11" s="2"/>
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
-      <c r="AV11" s="2"/>
+      <c r="AV11" s="48"/>
       <c r="AW11" s="2"/>
       <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
@@ -1879,34 +1917,32 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
+      <c r="AD12" s="48"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
+      <c r="AJ12" s="48"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
-      <c r="AP12" s="2"/>
+      <c r="AP12" s="48"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
       <c r="AS12" s="2"/>
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
-      <c r="AV12" s="2"/>
+      <c r="AV12" s="48"/>
       <c r="AW12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
       <c r="AZ12" s="43"/>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
-        <v>53</v>
-      </c>
+      <c r="A13" s="40"/>
       <c r="B13" s="32"/>
       <c r="C13" s="11" t="s">
         <v>61</v>
@@ -1937,94 +1973,92 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
+      <c r="AD13" s="48"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
+      <c r="AJ13" s="48"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
+      <c r="AP13" s="48"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
       <c r="AS13" s="2"/>
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
-      <c r="AV13" s="2"/>
+      <c r="AV13" s="48"/>
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="43"/>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="24"/>
-      <c r="AD14" s="24"/>
-      <c r="AE14" s="24"/>
-      <c r="AF14" s="24"/>
-      <c r="AG14" s="24"/>
-      <c r="AH14" s="24"/>
-      <c r="AI14" s="24"/>
-      <c r="AJ14" s="24"/>
-      <c r="AK14" s="24"/>
-      <c r="AL14" s="24"/>
-      <c r="AM14" s="24"/>
-      <c r="AN14" s="24"/>
-      <c r="AO14" s="24"/>
-      <c r="AP14" s="24"/>
-      <c r="AQ14" s="24"/>
-      <c r="AR14" s="24"/>
-      <c r="AS14" s="24"/>
-      <c r="AT14" s="24"/>
-      <c r="AU14" s="24"/>
-      <c r="AV14" s="24"/>
-      <c r="AW14" s="24"/>
-      <c r="AX14" s="24"/>
-      <c r="AY14" s="24"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="48"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="48"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="48"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="48"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
       <c r="AZ14" s="43"/>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="11"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="D15" s="12"/>
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
@@ -2035,9 +2069,8 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="N15" s="45"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -2051,41 +2084,37 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
+      <c r="AD15" s="48"/>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
+      <c r="AJ15" s="48"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
-      <c r="AP15" s="2"/>
+      <c r="AP15" s="48"/>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2"/>
       <c r="AS15" s="2"/>
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
-      <c r="AV15" s="2"/>
+      <c r="AV15" s="48"/>
       <c r="AW15" s="2"/>
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
       <c r="AZ15" s="43"/>
     </row>
-    <row r="16" spans="1:52" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
-        <v>62</v>
-      </c>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
       <c r="B16" s="32"/>
       <c r="C16" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>93</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="4"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -2095,9 +2124,8 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="N16" s="45"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -2111,41 +2139,39 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
+      <c r="AD16" s="48"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
-      <c r="AJ16" s="2"/>
+      <c r="AJ16" s="48"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
-      <c r="AP16" s="2"/>
+      <c r="AP16" s="48"/>
       <c r="AQ16" s="2"/>
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
-      <c r="AV16" s="2"/>
+      <c r="AV16" s="48"/>
       <c r="AW16" s="2"/>
       <c r="AX16" s="2"/>
       <c r="AY16" s="2"/>
       <c r="AZ16" s="43"/>
     </row>
-    <row r="17" spans="1:52" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B17" s="32"/>
-      <c r="C17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C17" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="4"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -2171,101 +2197,95 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
+      <c r="AD17" s="48"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
+      <c r="AJ17" s="48"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
-      <c r="AP17" s="2"/>
+      <c r="AP17" s="48"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
       <c r="AS17" s="2"/>
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
-      <c r="AV17" s="2"/>
+      <c r="AV17" s="48"/>
       <c r="AW17" s="2"/>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="43"/>
     </row>
-    <row r="18" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="2"/>
-      <c r="AN18" s="2"/>
-      <c r="AO18" s="2"/>
-      <c r="AP18" s="2"/>
-      <c r="AQ18" s="2"/>
-      <c r="AR18" s="2"/>
-      <c r="AS18" s="2"/>
-      <c r="AT18" s="2"/>
-      <c r="AU18" s="2"/>
-      <c r="AV18" s="2"/>
-      <c r="AW18" s="2"/>
-      <c r="AX18" s="2"/>
-      <c r="AY18" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+      <c r="AG18" s="24"/>
+      <c r="AH18" s="24"/>
+      <c r="AI18" s="24"/>
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="24"/>
+      <c r="AL18" s="24"/>
+      <c r="AM18" s="24"/>
+      <c r="AN18" s="24"/>
+      <c r="AO18" s="24"/>
+      <c r="AP18" s="48"/>
+      <c r="AQ18" s="24"/>
+      <c r="AR18" s="24"/>
+      <c r="AS18" s="24"/>
+      <c r="AT18" s="24"/>
+      <c r="AU18" s="24"/>
+      <c r="AV18" s="48"/>
+      <c r="AW18" s="24"/>
+      <c r="AX18" s="24"/>
+      <c r="AY18" s="24"/>
       <c r="AZ18" s="43"/>
     </row>
-    <row r="19" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>72</v>
-      </c>
+      <c r="B19" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2291,39 +2311,41 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
+      <c r="AD19" s="48"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
+      <c r="AJ19" s="48"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
-      <c r="AP19" s="2"/>
+      <c r="AP19" s="48"/>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
       <c r="AS19" s="2"/>
       <c r="AT19" s="2"/>
       <c r="AU19" s="2"/>
-      <c r="AV19" s="2"/>
+      <c r="AV19" s="48"/>
       <c r="AW19" s="2"/>
       <c r="AX19" s="2"/>
       <c r="AY19" s="2"/>
       <c r="AZ19" s="43"/>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2349,40 +2371,40 @@
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
+      <c r="AD20" s="48"/>
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
+      <c r="AJ20" s="48"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
-      <c r="AP20" s="2"/>
+      <c r="AP20" s="48"/>
       <c r="AQ20" s="2"/>
       <c r="AR20" s="2"/>
       <c r="AS20" s="2"/>
       <c r="AT20" s="2"/>
       <c r="AU20" s="2"/>
-      <c r="AV20" s="2"/>
+      <c r="AV20" s="48"/>
       <c r="AW20" s="2"/>
       <c r="AX20" s="2"/>
       <c r="AY20" s="2"/>
       <c r="AZ20" s="43"/>
     </row>
-    <row r="21" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="32"/>
       <c r="C21" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="2"/>
@@ -2409,39 +2431,41 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="2"/>
+      <c r="AD21" s="48"/>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="2"/>
+      <c r="AJ21" s="48"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
-      <c r="AP21" s="2"/>
+      <c r="AP21" s="48"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
       <c r="AS21" s="2"/>
       <c r="AT21" s="2"/>
       <c r="AU21" s="2"/>
-      <c r="AV21" s="2"/>
+      <c r="AV21" s="48"/>
       <c r="AW21" s="2"/>
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
       <c r="AZ21" s="43"/>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -2467,40 +2491,40 @@
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
-      <c r="AD22" s="2"/>
+      <c r="AD22" s="48"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
-      <c r="AJ22" s="2"/>
+      <c r="AJ22" s="48"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
-      <c r="AP22" s="2"/>
+      <c r="AP22" s="48"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2"/>
       <c r="AS22" s="2"/>
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
-      <c r="AV22" s="2"/>
+      <c r="AV22" s="48"/>
       <c r="AW22" s="2"/>
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
       <c r="AZ22" s="43"/>
     </row>
-    <row r="23" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -2527,41 +2551,39 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="2"/>
+      <c r="AD23" s="48"/>
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="2"/>
+      <c r="AJ23" s="48"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="2"/>
+      <c r="AP23" s="48"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
-      <c r="AV23" s="2"/>
+      <c r="AV23" s="48"/>
       <c r="AW23" s="2"/>
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
       <c r="AZ23" s="43"/>
     </row>
-    <row r="24" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B24" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2587,25 +2609,25 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
-      <c r="AD24" s="2"/>
+      <c r="AD24" s="48"/>
       <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
-      <c r="AJ24" s="2"/>
+      <c r="AJ24" s="48"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
-      <c r="AP24" s="2"/>
+      <c r="AP24" s="48"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
       <c r="AS24" s="2"/>
       <c r="AT24" s="2"/>
       <c r="AU24" s="2"/>
-      <c r="AV24" s="2"/>
+      <c r="AV24" s="48"/>
       <c r="AW24" s="2"/>
       <c r="AX24" s="2"/>
       <c r="AY24" s="2"/>
@@ -2617,10 +2639,10 @@
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
@@ -2647,41 +2669,39 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="2"/>
+      <c r="AD25" s="48"/>
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="2"/>
+      <c r="AJ25" s="48"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
-      <c r="AP25" s="2"/>
+      <c r="AP25" s="48"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
       <c r="AS25" s="2"/>
       <c r="AT25" s="2"/>
       <c r="AU25" s="2"/>
-      <c r="AV25" s="2"/>
+      <c r="AV25" s="48"/>
       <c r="AW25" s="2"/>
       <c r="AX25" s="2"/>
       <c r="AY25" s="2"/>
       <c r="AZ25" s="43"/>
     </row>
-    <row r="26" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>96</v>
-      </c>
+      <c r="B26" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="4"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2707,95 +2727,101 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="2"/>
+      <c r="AD26" s="48"/>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="2"/>
+      <c r="AJ26" s="48"/>
       <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
-      <c r="AP26" s="2"/>
+      <c r="AP26" s="48"/>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
       <c r="AS26" s="2"/>
       <c r="AT26" s="2"/>
       <c r="AU26" s="2"/>
-      <c r="AV26" s="2"/>
+      <c r="AV26" s="48"/>
       <c r="AW26" s="2"/>
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
       <c r="AZ26" s="43"/>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AB27" s="24"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="24"/>
-      <c r="AG27" s="24"/>
-      <c r="AH27" s="24"/>
-      <c r="AI27" s="24"/>
-      <c r="AJ27" s="24"/>
-      <c r="AK27" s="24"/>
-      <c r="AL27" s="24"/>
-      <c r="AM27" s="24"/>
-      <c r="AN27" s="24"/>
-      <c r="AO27" s="24"/>
-      <c r="AP27" s="24"/>
-      <c r="AQ27" s="24"/>
-      <c r="AR27" s="24"/>
-      <c r="AS27" s="24"/>
-      <c r="AT27" s="24"/>
-      <c r="AU27" s="24"/>
-      <c r="AV27" s="24"/>
-      <c r="AW27" s="24"/>
-      <c r="AX27" s="24"/>
-      <c r="AY27" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="48"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="48"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+      <c r="AP27" s="48"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="48"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="2"/>
       <c r="AZ27" s="43"/>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="E28" s="4"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2821,39 +2847,41 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
-      <c r="AD28" s="2"/>
+      <c r="AD28" s="48"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
-      <c r="AJ28" s="2"/>
+      <c r="AJ28" s="48"/>
       <c r="AK28" s="2"/>
       <c r="AL28" s="2"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
-      <c r="AP28" s="2"/>
+      <c r="AP28" s="48"/>
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
       <c r="AS28" s="2"/>
       <c r="AT28" s="2"/>
       <c r="AU28" s="2"/>
-      <c r="AV28" s="2"/>
+      <c r="AV28" s="48"/>
       <c r="AW28" s="2"/>
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
       <c r="AZ28" s="43"/>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B29" s="32"/>
       <c r="C29" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="E29" s="4"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2879,39 +2907,41 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="2"/>
+      <c r="AD29" s="48"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
-      <c r="AJ29" s="2"/>
+      <c r="AJ29" s="48"/>
       <c r="AK29" s="2"/>
       <c r="AL29" s="2"/>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
-      <c r="AP29" s="2"/>
+      <c r="AP29" s="48"/>
       <c r="AQ29" s="2"/>
       <c r="AR29" s="2"/>
       <c r="AS29" s="2"/>
       <c r="AT29" s="2"/>
       <c r="AU29" s="2"/>
-      <c r="AV29" s="2"/>
+      <c r="AV29" s="48"/>
       <c r="AW29" s="2"/>
       <c r="AX29" s="2"/>
       <c r="AY29" s="2"/>
       <c r="AZ29" s="43"/>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2937,25 +2967,25 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
-      <c r="AD30" s="2"/>
+      <c r="AD30" s="48"/>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
-      <c r="AJ30" s="2"/>
+      <c r="AJ30" s="48"/>
       <c r="AK30" s="2"/>
       <c r="AL30" s="2"/>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
-      <c r="AP30" s="2"/>
+      <c r="AP30" s="48"/>
       <c r="AQ30" s="2"/>
       <c r="AR30" s="2"/>
       <c r="AS30" s="2"/>
       <c r="AT30" s="2"/>
       <c r="AU30" s="2"/>
-      <c r="AV30" s="2"/>
+      <c r="AV30" s="48"/>
       <c r="AW30" s="2"/>
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
@@ -2963,60 +2993,58 @@
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-      <c r="AA31" s="2"/>
-      <c r="AB31" s="2"/>
-      <c r="AC31" s="2"/>
-      <c r="AD31" s="2"/>
-      <c r="AE31" s="2"/>
-      <c r="AF31" s="2"/>
-      <c r="AG31" s="2"/>
-      <c r="AH31" s="2"/>
-      <c r="AI31" s="2"/>
-      <c r="AJ31" s="2"/>
-      <c r="AK31" s="2"/>
-      <c r="AL31" s="2"/>
-      <c r="AM31" s="2"/>
-      <c r="AN31" s="2"/>
-      <c r="AO31" s="2"/>
-      <c r="AP31" s="2"/>
-      <c r="AQ31" s="2"/>
-      <c r="AR31" s="2"/>
-      <c r="AS31" s="2"/>
-      <c r="AT31" s="2"/>
-      <c r="AU31" s="2"/>
-      <c r="AV31" s="2"/>
-      <c r="AW31" s="2"/>
-      <c r="AX31" s="2"/>
-      <c r="AY31" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="24"/>
+      <c r="X31" s="24"/>
+      <c r="Y31" s="24"/>
+      <c r="Z31" s="24"/>
+      <c r="AA31" s="24"/>
+      <c r="AB31" s="24"/>
+      <c r="AC31" s="24"/>
+      <c r="AD31" s="48"/>
+      <c r="AE31" s="24"/>
+      <c r="AF31" s="24"/>
+      <c r="AG31" s="24"/>
+      <c r="AH31" s="24"/>
+      <c r="AI31" s="24"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="24"/>
+      <c r="AL31" s="24"/>
+      <c r="AM31" s="24"/>
+      <c r="AN31" s="24"/>
+      <c r="AO31" s="24"/>
+      <c r="AP31" s="48"/>
+      <c r="AQ31" s="24"/>
+      <c r="AR31" s="24"/>
+      <c r="AS31" s="24"/>
+      <c r="AT31" s="24"/>
+      <c r="AU31" s="24"/>
+      <c r="AV31" s="48"/>
+      <c r="AW31" s="24"/>
+      <c r="AX31" s="24"/>
+      <c r="AY31" s="24"/>
       <c r="AZ31" s="43"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
@@ -3024,7 +3052,7 @@
         <v>79</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
@@ -3053,25 +3081,25 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-      <c r="AD32" s="2"/>
+      <c r="AD32" s="48"/>
       <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
-      <c r="AJ32" s="2"/>
+      <c r="AJ32" s="48"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
-      <c r="AP32" s="2"/>
+      <c r="AP32" s="48"/>
       <c r="AQ32" s="2"/>
       <c r="AR32" s="2"/>
       <c r="AS32" s="2"/>
       <c r="AT32" s="2"/>
       <c r="AU32" s="2"/>
-      <c r="AV32" s="2"/>
+      <c r="AV32" s="48"/>
       <c r="AW32" s="2"/>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
@@ -3083,7 +3111,7 @@
       </c>
       <c r="B33" s="32"/>
       <c r="C33" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="4"/>
@@ -3111,25 +3139,25 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-      <c r="AD33" s="2"/>
+      <c r="AD33" s="48"/>
       <c r="AE33" s="2"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
-      <c r="AJ33" s="2"/>
+      <c r="AJ33" s="48"/>
       <c r="AK33" s="2"/>
       <c r="AL33" s="2"/>
       <c r="AM33" s="2"/>
       <c r="AN33" s="2"/>
       <c r="AO33" s="2"/>
-      <c r="AP33" s="2"/>
+      <c r="AP33" s="48"/>
       <c r="AQ33" s="2"/>
       <c r="AR33" s="2"/>
       <c r="AS33" s="2"/>
       <c r="AT33" s="2"/>
       <c r="AU33" s="2"/>
-      <c r="AV33" s="2"/>
+      <c r="AV33" s="48"/>
       <c r="AW33" s="2"/>
       <c r="AX33" s="2"/>
       <c r="AY33" s="2"/>
@@ -3139,10 +3167,10 @@
       <c r="A34" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="11"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="D34" s="12"/>
       <c r="E34" s="4"/>
       <c r="F34" s="2"/>
@@ -3169,25 +3197,25 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="2"/>
+      <c r="AD34" s="48"/>
       <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="2"/>
+      <c r="AJ34" s="48"/>
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
       <c r="AO34" s="2"/>
-      <c r="AP34" s="2"/>
+      <c r="AP34" s="48"/>
       <c r="AQ34" s="2"/>
       <c r="AR34" s="2"/>
       <c r="AS34" s="2"/>
       <c r="AT34" s="2"/>
       <c r="AU34" s="2"/>
-      <c r="AV34" s="2"/>
+      <c r="AV34" s="48"/>
       <c r="AW34" s="2"/>
       <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
@@ -3199,7 +3227,7 @@
       </c>
       <c r="B35" s="32"/>
       <c r="C35" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="4"/>
@@ -3227,25 +3255,25 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
-      <c r="AD35" s="2"/>
+      <c r="AD35" s="48"/>
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
-      <c r="AJ35" s="2"/>
+      <c r="AJ35" s="48"/>
       <c r="AK35" s="2"/>
       <c r="AL35" s="2"/>
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
       <c r="AO35" s="2"/>
-      <c r="AP35" s="2"/>
+      <c r="AP35" s="48"/>
       <c r="AQ35" s="2"/>
       <c r="AR35" s="2"/>
       <c r="AS35" s="2"/>
       <c r="AT35" s="2"/>
       <c r="AU35" s="2"/>
-      <c r="AV35" s="2"/>
+      <c r="AV35" s="48"/>
       <c r="AW35" s="2"/>
       <c r="AX35" s="2"/>
       <c r="AY35" s="2"/>
@@ -3255,10 +3283,10 @@
       <c r="A36" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="B36" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="11"/>
       <c r="D36" s="12"/>
       <c r="E36" s="4"/>
       <c r="F36" s="2"/>
@@ -3285,25 +3313,25 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="2"/>
+      <c r="AD36" s="48"/>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
-      <c r="AJ36" s="2"/>
+      <c r="AJ36" s="48"/>
       <c r="AK36" s="2"/>
       <c r="AL36" s="2"/>
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
       <c r="AO36" s="2"/>
-      <c r="AP36" s="2"/>
+      <c r="AP36" s="48"/>
       <c r="AQ36" s="2"/>
       <c r="AR36" s="2"/>
       <c r="AS36" s="2"/>
       <c r="AT36" s="2"/>
       <c r="AU36" s="2"/>
-      <c r="AV36" s="2"/>
+      <c r="AV36" s="48"/>
       <c r="AW36" s="2"/>
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
@@ -3315,7 +3343,7 @@
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="4"/>
@@ -3343,25 +3371,25 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
-      <c r="AD37" s="2"/>
+      <c r="AD37" s="48"/>
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
-      <c r="AJ37" s="2"/>
+      <c r="AJ37" s="48"/>
       <c r="AK37" s="2"/>
       <c r="AL37" s="2"/>
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
-      <c r="AP37" s="2"/>
+      <c r="AP37" s="48"/>
       <c r="AQ37" s="2"/>
       <c r="AR37" s="2"/>
       <c r="AS37" s="2"/>
       <c r="AT37" s="2"/>
       <c r="AU37" s="2"/>
-      <c r="AV37" s="2"/>
+      <c r="AV37" s="48"/>
       <c r="AW37" s="2"/>
       <c r="AX37" s="2"/>
       <c r="AY37" s="2"/>
@@ -3369,293 +3397,299 @@
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
-      <c r="P38" s="28"/>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="28"/>
-      <c r="S38" s="28"/>
-      <c r="T38" s="28"/>
-      <c r="U38" s="28"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
-      <c r="Y38" s="28"/>
-      <c r="Z38" s="28"/>
-      <c r="AA38" s="28"/>
-      <c r="AB38" s="28"/>
-      <c r="AC38" s="28"/>
-      <c r="AD38" s="28"/>
-      <c r="AE38" s="28"/>
-      <c r="AF38" s="28"/>
-      <c r="AG38" s="28"/>
-      <c r="AH38" s="28"/>
-      <c r="AI38" s="28"/>
-      <c r="AJ38" s="28"/>
-      <c r="AK38" s="28"/>
-      <c r="AL38" s="28"/>
-      <c r="AM38" s="28"/>
-      <c r="AN38" s="28"/>
-      <c r="AO38" s="28"/>
-      <c r="AP38" s="28"/>
-      <c r="AQ38" s="28"/>
-      <c r="AR38" s="28"/>
-      <c r="AS38" s="28"/>
-      <c r="AT38" s="28"/>
-      <c r="AU38" s="28"/>
-      <c r="AV38" s="28"/>
-      <c r="AW38" s="28"/>
-      <c r="AX38" s="28"/>
-      <c r="AY38" s="28"/>
+        <v>79</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="48"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AI38" s="2"/>
+      <c r="AJ38" s="48"/>
+      <c r="AK38" s="2"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+      <c r="AP38" s="48"/>
+      <c r="AQ38" s="2"/>
+      <c r="AR38" s="2"/>
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+      <c r="AV38" s="48"/>
+      <c r="AW38" s="2"/>
+      <c r="AX38" s="2"/>
+      <c r="AY38" s="2"/>
       <c r="AZ38" s="43"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="3"/>
-      <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="3"/>
-      <c r="AG39" s="3"/>
-      <c r="AH39" s="3"/>
-      <c r="AI39" s="3"/>
-      <c r="AJ39" s="3"/>
-      <c r="AK39" s="3"/>
-      <c r="AL39" s="3"/>
-      <c r="AM39" s="3"/>
-      <c r="AN39" s="3"/>
-      <c r="AO39" s="3"/>
-      <c r="AP39" s="3"/>
-      <c r="AQ39" s="3"/>
-      <c r="AR39" s="3"/>
-      <c r="AS39" s="3"/>
-      <c r="AT39" s="3"/>
-      <c r="AU39" s="3"/>
-      <c r="AV39" s="3"/>
-      <c r="AW39" s="3"/>
-      <c r="AX39" s="3"/>
-      <c r="AY39" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="48"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AI39" s="2"/>
+      <c r="AJ39" s="48"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="48"/>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="2"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="48"/>
+      <c r="AW39" s="2"/>
+      <c r="AX39" s="2"/>
+      <c r="AY39" s="2"/>
       <c r="AZ39" s="43"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="3"/>
-      <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
-      <c r="AF40" s="3"/>
-      <c r="AG40" s="3"/>
-      <c r="AH40" s="3"/>
-      <c r="AI40" s="3"/>
-      <c r="AJ40" s="3"/>
-      <c r="AK40" s="3"/>
-      <c r="AL40" s="3"/>
-      <c r="AM40" s="3"/>
-      <c r="AN40" s="3"/>
-      <c r="AO40" s="3"/>
-      <c r="AP40" s="3"/>
-      <c r="AQ40" s="3"/>
-      <c r="AR40" s="3"/>
-      <c r="AS40" s="3"/>
-      <c r="AT40" s="3"/>
-      <c r="AU40" s="3"/>
-      <c r="AV40" s="3"/>
-      <c r="AW40" s="3"/>
-      <c r="AX40" s="3"/>
-      <c r="AY40" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="48"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AI40" s="2"/>
+      <c r="AJ40" s="48"/>
+      <c r="AK40" s="2"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="48"/>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="2"/>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="2"/>
+      <c r="AV40" s="48"/>
+      <c r="AW40" s="2"/>
+      <c r="AX40" s="2"/>
+      <c r="AY40" s="2"/>
       <c r="AZ40" s="43"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AA41" s="3"/>
-      <c r="AB41" s="3"/>
-      <c r="AC41" s="3"/>
-      <c r="AD41" s="3"/>
-      <c r="AE41" s="3"/>
-      <c r="AF41" s="3"/>
-      <c r="AG41" s="3"/>
-      <c r="AH41" s="3"/>
-      <c r="AI41" s="3"/>
-      <c r="AJ41" s="3"/>
-      <c r="AK41" s="3"/>
-      <c r="AL41" s="3"/>
-      <c r="AM41" s="3"/>
-      <c r="AN41" s="3"/>
-      <c r="AO41" s="3"/>
-      <c r="AP41" s="3"/>
-      <c r="AQ41" s="3"/>
-      <c r="AR41" s="3"/>
-      <c r="AS41" s="3"/>
-      <c r="AT41" s="3"/>
-      <c r="AU41" s="3"/>
-      <c r="AV41" s="3"/>
-      <c r="AW41" s="3"/>
-      <c r="AX41" s="3"/>
-      <c r="AY41" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="48"/>
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+      <c r="AG41" s="2"/>
+      <c r="AH41" s="2"/>
+      <c r="AI41" s="2"/>
+      <c r="AJ41" s="48"/>
+      <c r="AK41" s="2"/>
+      <c r="AL41" s="2"/>
+      <c r="AM41" s="2"/>
+      <c r="AN41" s="2"/>
+      <c r="AO41" s="2"/>
+      <c r="AP41" s="48"/>
+      <c r="AQ41" s="2"/>
+      <c r="AR41" s="2"/>
+      <c r="AS41" s="2"/>
+      <c r="AT41" s="2"/>
+      <c r="AU41" s="2"/>
+      <c r="AV41" s="48"/>
+      <c r="AW41" s="2"/>
+      <c r="AX41" s="2"/>
+      <c r="AY41" s="2"/>
       <c r="AZ41" s="43"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="3"/>
-      <c r="AG42" s="3"/>
-      <c r="AH42" s="3"/>
-      <c r="AI42" s="3"/>
-      <c r="AJ42" s="3"/>
-      <c r="AK42" s="3"/>
-      <c r="AL42" s="3"/>
-      <c r="AM42" s="3"/>
-      <c r="AN42" s="3"/>
-      <c r="AO42" s="3"/>
-      <c r="AP42" s="3"/>
-      <c r="AQ42" s="3"/>
-      <c r="AR42" s="3"/>
-      <c r="AS42" s="3"/>
-      <c r="AT42" s="3"/>
-      <c r="AU42" s="3"/>
-      <c r="AV42" s="3"/>
-      <c r="AW42" s="3"/>
-      <c r="AX42" s="3"/>
-      <c r="AY42" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="B42" s="34"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="28"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="28"/>
+      <c r="AB42" s="28"/>
+      <c r="AC42" s="28"/>
+      <c r="AD42" s="49"/>
+      <c r="AE42" s="28"/>
+      <c r="AF42" s="28"/>
+      <c r="AG42" s="28"/>
+      <c r="AH42" s="28"/>
+      <c r="AI42" s="28"/>
+      <c r="AJ42" s="49"/>
+      <c r="AK42" s="28"/>
+      <c r="AL42" s="28"/>
+      <c r="AM42" s="28"/>
+      <c r="AN42" s="28"/>
+      <c r="AO42" s="28"/>
+      <c r="AP42" s="49"/>
+      <c r="AQ42" s="28"/>
+      <c r="AR42" s="28"/>
+      <c r="AS42" s="28"/>
+      <c r="AT42" s="28"/>
+      <c r="AU42" s="28"/>
+      <c r="AV42" s="49"/>
+      <c r="AW42" s="28"/>
+      <c r="AX42" s="28"/>
+      <c r="AY42" s="28"/>
       <c r="AZ42" s="43"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="35" t="s">
+        <v>3</v>
+      </c>
       <c r="C43" s="10"/>
       <c r="D43" s="13"/>
       <c r="E43" s="5"/>
@@ -3683,25 +3717,25 @@
       <c r="AA43" s="3"/>
       <c r="AB43" s="3"/>
       <c r="AC43" s="3"/>
-      <c r="AD43" s="3"/>
+      <c r="AD43" s="49"/>
       <c r="AE43" s="3"/>
       <c r="AF43" s="3"/>
       <c r="AG43" s="3"/>
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
-      <c r="AJ43" s="3"/>
+      <c r="AJ43" s="49"/>
       <c r="AK43" s="3"/>
       <c r="AL43" s="3"/>
       <c r="AM43" s="3"/>
       <c r="AN43" s="3"/>
       <c r="AO43" s="3"/>
-      <c r="AP43" s="3"/>
+      <c r="AP43" s="49"/>
       <c r="AQ43" s="3"/>
       <c r="AR43" s="3"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
       <c r="AU43" s="3"/>
-      <c r="AV43" s="3"/>
+      <c r="AV43" s="49"/>
       <c r="AW43" s="3"/>
       <c r="AX43" s="3"/>
       <c r="AY43" s="3"/>
@@ -3739,39 +3773,37 @@
       <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
-      <c r="AD44" s="3"/>
+      <c r="AD44" s="49"/>
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
-      <c r="AJ44" s="3"/>
+      <c r="AJ44" s="49"/>
       <c r="AK44" s="3"/>
       <c r="AL44" s="3"/>
       <c r="AM44" s="3"/>
       <c r="AN44" s="3"/>
       <c r="AO44" s="3"/>
-      <c r="AP44" s="3"/>
+      <c r="AP44" s="49"/>
       <c r="AQ44" s="3"/>
       <c r="AR44" s="3"/>
       <c r="AS44" s="3"/>
       <c r="AT44" s="3"/>
       <c r="AU44" s="3"/>
-      <c r="AV44" s="3"/>
+      <c r="AV44" s="49"/>
       <c r="AW44" s="3"/>
       <c r="AX44" s="3"/>
       <c r="AY44" s="3"/>
       <c r="AZ44" s="43"/>
     </row>
-    <row r="45" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="41" t="s">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A45" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="16"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="13"/>
       <c r="E45" s="5"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -3797,34 +3829,262 @@
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
-      <c r="AD45" s="3"/>
+      <c r="AD45" s="49"/>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
-      <c r="AJ45" s="3"/>
+      <c r="AJ45" s="49"/>
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
       <c r="AN45" s="3"/>
       <c r="AO45" s="3"/>
-      <c r="AP45" s="3"/>
+      <c r="AP45" s="49"/>
       <c r="AQ45" s="3"/>
       <c r="AR45" s="3"/>
       <c r="AS45" s="3"/>
       <c r="AT45" s="3"/>
       <c r="AU45" s="3"/>
-      <c r="AV45" s="3"/>
+      <c r="AV45" s="49"/>
       <c r="AW45" s="3"/>
       <c r="AX45" s="3"/>
       <c r="AY45" s="3"/>
-      <c r="AZ45" s="44"/>
-    </row>
-    <row r="46" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="AZ45" s="43"/>
+    </row>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A46" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3"/>
+      <c r="AC46" s="3"/>
+      <c r="AD46" s="49"/>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
+      <c r="AG46" s="3"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="3"/>
+      <c r="AJ46" s="49"/>
+      <c r="AK46" s="3"/>
+      <c r="AL46" s="3"/>
+      <c r="AM46" s="3"/>
+      <c r="AN46" s="3"/>
+      <c r="AO46" s="3"/>
+      <c r="AP46" s="49"/>
+      <c r="AQ46" s="3"/>
+      <c r="AR46" s="3"/>
+      <c r="AS46" s="3"/>
+      <c r="AT46" s="3"/>
+      <c r="AU46" s="3"/>
+      <c r="AV46" s="49"/>
+      <c r="AW46" s="3"/>
+      <c r="AX46" s="3"/>
+      <c r="AY46" s="3"/>
+      <c r="AZ46" s="43"/>
+    </row>
+    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A47" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="32"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+      <c r="AA47" s="3"/>
+      <c r="AB47" s="3"/>
+      <c r="AC47" s="3"/>
+      <c r="AD47" s="49"/>
+      <c r="AE47" s="3"/>
+      <c r="AF47" s="3"/>
+      <c r="AG47" s="3"/>
+      <c r="AH47" s="3"/>
+      <c r="AI47" s="3"/>
+      <c r="AJ47" s="49"/>
+      <c r="AK47" s="3"/>
+      <c r="AL47" s="3"/>
+      <c r="AM47" s="3"/>
+      <c r="AN47" s="3"/>
+      <c r="AO47" s="3"/>
+      <c r="AP47" s="49"/>
+      <c r="AQ47" s="3"/>
+      <c r="AR47" s="3"/>
+      <c r="AS47" s="3"/>
+      <c r="AT47" s="3"/>
+      <c r="AU47" s="3"/>
+      <c r="AV47" s="49"/>
+      <c r="AW47" s="3"/>
+      <c r="AX47" s="3"/>
+      <c r="AY47" s="3"/>
+      <c r="AZ47" s="43"/>
+    </row>
+    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A48" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="35"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3"/>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="49"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="49"/>
+      <c r="AK48" s="3"/>
+      <c r="AL48" s="3"/>
+      <c r="AM48" s="3"/>
+      <c r="AN48" s="3"/>
+      <c r="AO48" s="3"/>
+      <c r="AP48" s="49"/>
+      <c r="AQ48" s="3"/>
+      <c r="AR48" s="3"/>
+      <c r="AS48" s="3"/>
+      <c r="AT48" s="3"/>
+      <c r="AU48" s="3"/>
+      <c r="AV48" s="49"/>
+      <c r="AW48" s="3"/>
+      <c r="AX48" s="3"/>
+      <c r="AY48" s="3"/>
+      <c r="AZ48" s="43"/>
+    </row>
+    <row r="49" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="3"/>
+      <c r="AC49" s="3"/>
+      <c r="AD49" s="49"/>
+      <c r="AE49" s="3"/>
+      <c r="AF49" s="3"/>
+      <c r="AG49" s="3"/>
+      <c r="AH49" s="3"/>
+      <c r="AI49" s="3"/>
+      <c r="AJ49" s="49"/>
+      <c r="AK49" s="3"/>
+      <c r="AL49" s="3"/>
+      <c r="AM49" s="3"/>
+      <c r="AN49" s="3"/>
+      <c r="AO49" s="3"/>
+      <c r="AP49" s="49"/>
+      <c r="AQ49" s="3"/>
+      <c r="AR49" s="3"/>
+      <c r="AS49" s="3"/>
+      <c r="AT49" s="3"/>
+      <c r="AU49" s="3"/>
+      <c r="AV49" s="49"/>
+      <c r="AW49" s="3"/>
+      <c r="AX49" s="3"/>
+      <c r="AY49" s="3"/>
+      <c r="AZ49" s="44"/>
+    </row>
+    <row r="50" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AZ2:AZ45"/>
+    <mergeCell ref="AZ2:AZ49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Docs(Add):changes to gantt-chart and gitignore + code example
</commit_message>
<xml_diff>
--- a/Dokumente/Planen/Projektablauf_Gantt.xlsx
+++ b/Dokumente/Planen/Projektablauf_Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/yves_jaros_edu_gbssg_ch/Documents/000_Schule_IMS-T1a/000_IMS/001-IntegriertePraxisarbeit/2025_TerminalChat/Dokumente/Planen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yvesj\source\2025_TerminalChat\Dokumente\Planen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{D7E4EBFE-A1CD-4CA4-901D-6FF22ED8BFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C34A6E9-E016-40CD-B22D-A6023E347A23}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94413C6A-6554-4E96-9FA7-2F017C038C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
   <si>
     <t>IPERKA</t>
   </si>
@@ -332,20 +332,32 @@
     <t>Code beispiel</t>
   </si>
   <si>
-    <t>Codebeispiel finden/ generieren</t>
-  </si>
-  <si>
     <t>Codebeispiel ausprobieren testen</t>
   </si>
   <si>
-    <t>Codebeispiel verstehen</t>
+    <t>TerminalChat</t>
+  </si>
+  <si>
+    <t>Projekt</t>
+  </si>
+  <si>
+    <t>IST</t>
+  </si>
+  <si>
+    <t>SOLL</t>
+  </si>
+  <si>
+    <t>Codebeispiel verstehen/dokumentieren</t>
+  </si>
+  <si>
+    <t>Codebeispiel finden/generieren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,8 +372,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,8 +417,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -707,11 +738,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -816,6 +860,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -825,19 +872,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1123,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ50"/>
+  <dimension ref="A2:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT20" sqref="AT20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AY50" sqref="AY50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,354 +1188,253 @@
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="15" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="13" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="10.7109375" customWidth="1"/>
     <col min="16" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="53" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="2" spans="1:52" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="29">
+      <c r="E3" s="29">
         <v>45719</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M3" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X3" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y3" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z3" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AW3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AX3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="AY3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="AZ3" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="4" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="47"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="47"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="47"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="42" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="47"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20"/>
+      <c r="AN4" s="20"/>
+      <c r="AO4" s="20"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="20"/>
+      <c r="AR4" s="20"/>
+      <c r="AS4" s="20"/>
+      <c r="AT4" s="20"/>
+      <c r="AU4" s="20"/>
+      <c r="AV4" s="47"/>
+      <c r="AW4" s="20"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="43" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="48"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="48"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="43"/>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-      <c r="AP4" s="48"/>
-      <c r="AQ4" s="2"/>
-      <c r="AR4" s="2"/>
-      <c r="AS4" s="2"/>
-      <c r="AT4" s="2"/>
-      <c r="AU4" s="2"/>
-      <c r="AV4" s="48"/>
-      <c r="AW4" s="2"/>
-      <c r="AX4" s="2"/>
-      <c r="AY4" s="2"/>
-      <c r="AZ4" s="43"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="12"/>
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
@@ -1493,9 +1445,9 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="42"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="45"/>
+      <c r="P5" s="42"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -1531,7 +1483,7 @@
       <c r="AW5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
-      <c r="AZ5" s="43"/>
+      <c r="AZ5" s="44"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -1539,7 +1491,7 @@
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="11" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="4"/>
@@ -1553,7 +1505,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="45"/>
+      <c r="P6" s="42"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -1589,17 +1541,17 @@
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
-      <c r="AZ6" s="43"/>
+      <c r="AZ6" s="44"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1611,7 +1563,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="42"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -1647,19 +1599,17 @@
       <c r="AW7" s="2"/>
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
-      <c r="AZ7" s="43"/>
-    </row>
-    <row r="8" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="AZ7" s="44"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>75</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D8" s="12"/>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1671,7 +1621,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="P8" s="42"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -1707,17 +1657,17 @@
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
-      <c r="AZ8" s="43"/>
+      <c r="AZ8" s="44"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1732,7 +1682,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="S9" s="42"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
@@ -1765,17 +1715,19 @@
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
-      <c r="AZ9" s="43"/>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ9" s="44"/>
+    </row>
+    <row r="10" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>56</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1790,7 +1742,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="S10" s="42"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
@@ -1823,16 +1775,16 @@
       <c r="AW10" s="2"/>
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
-      <c r="AZ10" s="43"/>
+      <c r="AZ10" s="44"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="B11" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="11"/>
       <c r="D11" s="12"/>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
@@ -1846,7 +1798,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="Q11" s="42"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -1881,16 +1833,16 @@
       <c r="AW11" s="2"/>
       <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
-      <c r="AZ11" s="43"/>
+      <c r="AZ11" s="44"/>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="11"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="D12" s="12"/>
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
@@ -1904,7 +1856,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
+      <c r="Q12" s="42"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
@@ -1939,13 +1891,15 @@
       <c r="AW12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
-      <c r="AZ12" s="43"/>
+      <c r="AZ12" s="44"/>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="40" t="s">
+        <v>53</v>
+      </c>
       <c r="B13" s="32"/>
       <c r="C13" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="4"/>
@@ -1960,7 +1914,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+      <c r="Q13" s="42"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
@@ -1995,12 +1949,14 @@
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
-      <c r="AZ13" s="43"/>
+      <c r="AZ13" s="44"/>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="40" t="s">
+        <v>53</v>
+      </c>
       <c r="B14" s="32" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
@@ -2017,7 +1973,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
+      <c r="R14" s="42"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
@@ -2051,13 +2007,15 @@
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
       <c r="AY14" s="2"/>
-      <c r="AZ14" s="43"/>
+      <c r="AZ14" s="44"/>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="40" t="s">
+        <v>53</v>
+      </c>
       <c r="B15" s="32"/>
       <c r="C15" s="11" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="4"/>
@@ -2069,10 +2027,11 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="45"/>
+      <c r="N15" s="2"/>
       <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="R15" s="42"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
@@ -2106,14 +2065,16 @@
       <c r="AW15" s="2"/>
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
-      <c r="AZ15" s="43"/>
+      <c r="AZ15" s="44"/>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="11" t="s">
-        <v>99</v>
-      </c>
+      <c r="A16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="12"/>
       <c r="E16" s="4"/>
       <c r="F16" s="2"/>
@@ -2124,8 +2085,9 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="45"/>
+      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -2161,15 +2123,15 @@
       <c r="AW16" s="2"/>
       <c r="AX16" s="2"/>
       <c r="AY16" s="2"/>
-      <c r="AZ16" s="43"/>
+      <c r="AZ16" s="44"/>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="32"/>
-      <c r="C17" s="46" t="s">
-        <v>100</v>
+      <c r="C17" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="4"/>
@@ -2181,9 +2143,9 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="N17" s="42"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="P17" s="3"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -2219,72 +2181,74 @@
       <c r="AW17" s="2"/>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
-      <c r="AZ17" s="43"/>
+      <c r="AZ17" s="44"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
+        <v>53</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
       <c r="AD18" s="48"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
-      <c r="AG18" s="24"/>
-      <c r="AH18" s="24"/>
-      <c r="AI18" s="24"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
       <c r="AJ18" s="48"/>
-      <c r="AK18" s="24"/>
-      <c r="AL18" s="24"/>
-      <c r="AM18" s="24"/>
-      <c r="AN18" s="24"/>
-      <c r="AO18" s="24"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
       <c r="AP18" s="48"/>
-      <c r="AQ18" s="24"/>
-      <c r="AR18" s="24"/>
-      <c r="AS18" s="24"/>
-      <c r="AT18" s="24"/>
-      <c r="AU18" s="24"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
       <c r="AV18" s="48"/>
-      <c r="AW18" s="24"/>
-      <c r="AX18" s="24"/>
-      <c r="AY18" s="24"/>
-      <c r="AZ18" s="43"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="44"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="11"/>
+        <v>53</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="D19" s="12"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
@@ -2301,16 +2265,16 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
+      <c r="T19" s="42"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="2"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="51"/>
       <c r="AD19" s="48"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
@@ -2333,79 +2297,73 @@
       <c r="AW19" s="2"/>
       <c r="AX19" s="2"/>
       <c r="AY19" s="2"/>
-      <c r="AZ19" s="43"/>
-    </row>
-    <row r="20" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="AZ19" s="44"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
       <c r="AD20" s="48"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2"/>
-      <c r="AI20" s="2"/>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="24"/>
+      <c r="AG20" s="24"/>
+      <c r="AH20" s="24"/>
+      <c r="AI20" s="24"/>
       <c r="AJ20" s="48"/>
-      <c r="AK20" s="2"/>
-      <c r="AL20" s="2"/>
-      <c r="AM20" s="2"/>
-      <c r="AN20" s="2"/>
-      <c r="AO20" s="2"/>
+      <c r="AK20" s="24"/>
+      <c r="AL20" s="24"/>
+      <c r="AM20" s="24"/>
+      <c r="AN20" s="24"/>
+      <c r="AO20" s="24"/>
       <c r="AP20" s="48"/>
-      <c r="AQ20" s="2"/>
-      <c r="AR20" s="2"/>
-      <c r="AS20" s="2"/>
-      <c r="AT20" s="2"/>
-      <c r="AU20" s="2"/>
+      <c r="AQ20" s="24"/>
+      <c r="AR20" s="24"/>
+      <c r="AS20" s="24"/>
+      <c r="AT20" s="24"/>
+      <c r="AU20" s="24"/>
       <c r="AV20" s="48"/>
-      <c r="AW20" s="2"/>
-      <c r="AX20" s="2"/>
-      <c r="AY20" s="2"/>
-      <c r="AZ20" s="43"/>
-    </row>
-    <row r="21" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="AW20" s="24"/>
+      <c r="AX20" s="24"/>
+      <c r="AY20" s="24"/>
+      <c r="AZ20" s="44"/>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="B21" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="4"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -2453,18 +2411,18 @@
       <c r="AW21" s="2"/>
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
-      <c r="AZ21" s="43"/>
-    </row>
-    <row r="22" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+      <c r="AZ21" s="44"/>
+    </row>
+    <row r="22" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B22" s="32"/>
       <c r="C22" s="11" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="2"/>
@@ -2492,7 +2450,7 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="48"/>
-      <c r="AE22" s="2"/>
+      <c r="AE22" s="51"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
@@ -2513,18 +2471,18 @@
       <c r="AW22" s="2"/>
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
-      <c r="AZ22" s="43"/>
-    </row>
-    <row r="23" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+      <c r="AZ22" s="44"/>
+    </row>
+    <row r="23" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -2552,7 +2510,7 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="48"/>
-      <c r="AE23" s="2"/>
+      <c r="AE23" s="51"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
@@ -2573,17 +2531,19 @@
       <c r="AW23" s="2"/>
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
-      <c r="AZ23" s="43"/>
-    </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ23" s="44"/>
+    </row>
+    <row r="24" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2611,7 +2571,7 @@
       <c r="AC24" s="2"/>
       <c r="AD24" s="48"/>
       <c r="AE24" s="2"/>
-      <c r="AF24" s="2"/>
+      <c r="AF24" s="51"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
@@ -2631,18 +2591,18 @@
       <c r="AW24" s="2"/>
       <c r="AX24" s="2"/>
       <c r="AY24" s="2"/>
-      <c r="AZ24" s="43"/>
-    </row>
-    <row r="25" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="AZ24" s="44"/>
+    </row>
+    <row r="25" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
@@ -2671,7 +2631,7 @@
       <c r="AC25" s="2"/>
       <c r="AD25" s="48"/>
       <c r="AE25" s="2"/>
-      <c r="AF25" s="2"/>
+      <c r="AF25" s="51"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
@@ -2691,14 +2651,14 @@
       <c r="AW25" s="2"/>
       <c r="AX25" s="2"/>
       <c r="AY25" s="2"/>
-      <c r="AZ25" s="43"/>
+      <c r="AZ25" s="44"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="12"/>
@@ -2749,18 +2709,18 @@
       <c r="AW26" s="2"/>
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
-      <c r="AZ26" s="43"/>
-    </row>
-    <row r="27" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="AZ26" s="44"/>
+    </row>
+    <row r="27" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="2"/>
@@ -2790,7 +2750,7 @@
       <c r="AD27" s="48"/>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
-      <c r="AG27" s="2"/>
+      <c r="AG27" s="51"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="48"/>
@@ -2809,19 +2769,17 @@
       <c r="AW27" s="2"/>
       <c r="AX27" s="2"/>
       <c r="AY27" s="2"/>
-      <c r="AZ27" s="43"/>
-    </row>
-    <row r="28" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="AZ27" s="44"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="B28" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="4"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2869,18 +2827,18 @@
       <c r="AW28" s="2"/>
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
-      <c r="AZ28" s="43"/>
-    </row>
-    <row r="29" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="AZ28" s="44"/>
+    </row>
+    <row r="29" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B29" s="32"/>
       <c r="C29" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="2"/>
@@ -2911,7 +2869,7 @@
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
-      <c r="AH29" s="2"/>
+      <c r="AH29" s="51"/>
       <c r="AI29" s="2"/>
       <c r="AJ29" s="48"/>
       <c r="AK29" s="2"/>
@@ -2929,18 +2887,18 @@
       <c r="AW29" s="2"/>
       <c r="AX29" s="2"/>
       <c r="AY29" s="2"/>
-      <c r="AZ29" s="43"/>
-    </row>
-    <row r="30" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+      <c r="AZ29" s="44"/>
+    </row>
+    <row r="30" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="2"/>
@@ -2971,7 +2929,7 @@
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
-      <c r="AH30" s="2"/>
+      <c r="AH30" s="51"/>
       <c r="AI30" s="2"/>
       <c r="AJ30" s="48"/>
       <c r="AK30" s="2"/>
@@ -2989,73 +2947,79 @@
       <c r="AW30" s="2"/>
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
-      <c r="AZ30" s="43"/>
-    </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ30" s="44"/>
+    </row>
+    <row r="31" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="24"/>
-      <c r="AC31" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
       <c r="AD31" s="48"/>
-      <c r="AE31" s="24"/>
-      <c r="AF31" s="24"/>
-      <c r="AG31" s="24"/>
-      <c r="AH31" s="24"/>
-      <c r="AI31" s="24"/>
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="51"/>
       <c r="AJ31" s="48"/>
-      <c r="AK31" s="24"/>
-      <c r="AL31" s="24"/>
-      <c r="AM31" s="24"/>
-      <c r="AN31" s="24"/>
-      <c r="AO31" s="24"/>
+      <c r="AK31" s="2"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="2"/>
+      <c r="AN31" s="2"/>
+      <c r="AO31" s="2"/>
       <c r="AP31" s="48"/>
-      <c r="AQ31" s="24"/>
-      <c r="AR31" s="24"/>
-      <c r="AS31" s="24"/>
-      <c r="AT31" s="24"/>
-      <c r="AU31" s="24"/>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="2"/>
+      <c r="AS31" s="2"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
       <c r="AV31" s="48"/>
-      <c r="AW31" s="24"/>
-      <c r="AX31" s="24"/>
-      <c r="AY31" s="24"/>
-      <c r="AZ31" s="43"/>
-    </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AW31" s="2"/>
+      <c r="AX31" s="2"/>
+      <c r="AY31" s="2"/>
+      <c r="AZ31" s="44"/>
+    </row>
+    <row r="32" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="B32" s="32"/>
+      <c r="C32" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>96</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -3086,7 +3050,7 @@
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
-      <c r="AI32" s="2"/>
+      <c r="AI32" s="51"/>
       <c r="AJ32" s="48"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
@@ -3103,74 +3067,72 @@
       <c r="AW32" s="2"/>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
-      <c r="AZ32" s="43"/>
+      <c r="AZ32" s="44"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-      <c r="AA33" s="2"/>
-      <c r="AB33" s="2"/>
-      <c r="AC33" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="24"/>
       <c r="AD33" s="48"/>
-      <c r="AE33" s="2"/>
-      <c r="AF33" s="2"/>
-      <c r="AG33" s="2"/>
-      <c r="AH33" s="2"/>
-      <c r="AI33" s="2"/>
+      <c r="AE33" s="24"/>
+      <c r="AF33" s="24"/>
+      <c r="AG33" s="24"/>
+      <c r="AH33" s="24"/>
+      <c r="AI33" s="24"/>
       <c r="AJ33" s="48"/>
-      <c r="AK33" s="2"/>
-      <c r="AL33" s="2"/>
-      <c r="AM33" s="2"/>
-      <c r="AN33" s="2"/>
-      <c r="AO33" s="2"/>
+      <c r="AK33" s="24"/>
+      <c r="AL33" s="24"/>
+      <c r="AM33" s="24"/>
+      <c r="AN33" s="24"/>
+      <c r="AO33" s="24"/>
       <c r="AP33" s="48"/>
-      <c r="AQ33" s="2"/>
-      <c r="AR33" s="2"/>
-      <c r="AS33" s="2"/>
-      <c r="AT33" s="2"/>
-      <c r="AU33" s="2"/>
+      <c r="AQ33" s="24"/>
+      <c r="AR33" s="24"/>
+      <c r="AS33" s="24"/>
+      <c r="AT33" s="24"/>
+      <c r="AU33" s="24"/>
       <c r="AV33" s="48"/>
-      <c r="AW33" s="2"/>
-      <c r="AX33" s="2"/>
-      <c r="AY33" s="2"/>
-      <c r="AZ33" s="43"/>
+      <c r="AW33" s="24"/>
+      <c r="AX33" s="24"/>
+      <c r="AY33" s="24"/>
+      <c r="AZ33" s="44"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="11" t="s">
-        <v>81</v>
-      </c>
+      <c r="B34" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="11"/>
       <c r="D34" s="12"/>
       <c r="E34" s="4"/>
       <c r="F34" s="2"/>
@@ -3204,7 +3166,7 @@
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
       <c r="AJ34" s="48"/>
-      <c r="AK34" s="2"/>
+      <c r="AK34" s="51"/>
       <c r="AL34" s="2"/>
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
@@ -3219,7 +3181,7 @@
       <c r="AW34" s="2"/>
       <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
-      <c r="AZ34" s="43"/>
+      <c r="AZ34" s="44"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
@@ -3227,7 +3189,7 @@
       </c>
       <c r="B35" s="32"/>
       <c r="C35" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="4"/>
@@ -3262,7 +3224,7 @@
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
       <c r="AJ35" s="48"/>
-      <c r="AK35" s="2"/>
+      <c r="AK35" s="51"/>
       <c r="AL35" s="2"/>
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
@@ -3277,16 +3239,16 @@
       <c r="AW35" s="2"/>
       <c r="AX35" s="2"/>
       <c r="AY35" s="2"/>
-      <c r="AZ35" s="43"/>
+      <c r="AZ35" s="44"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="11"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="D36" s="12"/>
       <c r="E36" s="4"/>
       <c r="F36" s="2"/>
@@ -3320,7 +3282,7 @@
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
       <c r="AJ36" s="48"/>
-      <c r="AK36" s="2"/>
+      <c r="AK36" s="51"/>
       <c r="AL36" s="2"/>
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
@@ -3335,7 +3297,7 @@
       <c r="AW36" s="2"/>
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
-      <c r="AZ36" s="43"/>
+      <c r="AZ36" s="44"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
@@ -3343,7 +3305,7 @@
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="4"/>
@@ -3379,7 +3341,7 @@
       <c r="AI37" s="2"/>
       <c r="AJ37" s="48"/>
       <c r="AK37" s="2"/>
-      <c r="AL37" s="2"/>
+      <c r="AL37" s="51"/>
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
@@ -3393,14 +3355,14 @@
       <c r="AW37" s="2"/>
       <c r="AX37" s="2"/>
       <c r="AY37" s="2"/>
-      <c r="AZ37" s="43"/>
+      <c r="AZ37" s="44"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>79</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="12"/>
@@ -3437,7 +3399,7 @@
       <c r="AI38" s="2"/>
       <c r="AJ38" s="48"/>
       <c r="AK38" s="2"/>
-      <c r="AL38" s="2"/>
+      <c r="AL38" s="51"/>
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
       <c r="AO38" s="2"/>
@@ -3451,7 +3413,7 @@
       <c r="AW38" s="2"/>
       <c r="AX38" s="2"/>
       <c r="AY38" s="2"/>
-      <c r="AZ38" s="43"/>
+      <c r="AZ38" s="44"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
@@ -3459,7 +3421,7 @@
       </c>
       <c r="B39" s="32"/>
       <c r="C39" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="4"/>
@@ -3496,7 +3458,7 @@
       <c r="AJ39" s="48"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="2"/>
-      <c r="AM39" s="2"/>
+      <c r="AM39" s="51"/>
       <c r="AN39" s="2"/>
       <c r="AO39" s="2"/>
       <c r="AP39" s="48"/>
@@ -3509,16 +3471,16 @@
       <c r="AW39" s="2"/>
       <c r="AX39" s="2"/>
       <c r="AY39" s="2"/>
-      <c r="AZ39" s="43"/>
+      <c r="AZ39" s="44"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="B40" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="11"/>
       <c r="D40" s="12"/>
       <c r="E40" s="4"/>
       <c r="F40" s="2"/>
@@ -3554,7 +3516,7 @@
       <c r="AJ40" s="48"/>
       <c r="AK40" s="2"/>
       <c r="AL40" s="2"/>
-      <c r="AM40" s="2"/>
+      <c r="AM40" s="51"/>
       <c r="AN40" s="2"/>
       <c r="AO40" s="2"/>
       <c r="AP40" s="48"/>
@@ -3567,7 +3529,7 @@
       <c r="AW40" s="2"/>
       <c r="AX40" s="2"/>
       <c r="AY40" s="2"/>
-      <c r="AZ40" s="43"/>
+      <c r="AZ40" s="44"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
@@ -3575,7 +3537,7 @@
       </c>
       <c r="B41" s="32"/>
       <c r="C41" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="4"/>
@@ -3612,7 +3574,7 @@
       <c r="AJ41" s="48"/>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
-      <c r="AM41" s="2"/>
+      <c r="AM41" s="51"/>
       <c r="AN41" s="2"/>
       <c r="AO41" s="2"/>
       <c r="AP41" s="48"/>
@@ -3625,183 +3587,187 @@
       <c r="AW41" s="2"/>
       <c r="AX41" s="2"/>
       <c r="AY41" s="2"/>
-      <c r="AZ41" s="43"/>
+      <c r="AZ41" s="44"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="28"/>
-      <c r="P42" s="28"/>
-      <c r="Q42" s="28"/>
-      <c r="R42" s="28"/>
-      <c r="S42" s="28"/>
-      <c r="T42" s="28"/>
-      <c r="U42" s="28"/>
-      <c r="V42" s="28"/>
-      <c r="W42" s="28"/>
-      <c r="X42" s="28"/>
-      <c r="Y42" s="28"/>
-      <c r="Z42" s="28"/>
-      <c r="AA42" s="28"/>
-      <c r="AB42" s="28"/>
-      <c r="AC42" s="28"/>
-      <c r="AD42" s="49"/>
-      <c r="AE42" s="28"/>
-      <c r="AF42" s="28"/>
-      <c r="AG42" s="28"/>
-      <c r="AH42" s="28"/>
-      <c r="AI42" s="28"/>
-      <c r="AJ42" s="49"/>
-      <c r="AK42" s="28"/>
-      <c r="AL42" s="28"/>
-      <c r="AM42" s="28"/>
-      <c r="AN42" s="28"/>
-      <c r="AO42" s="28"/>
-      <c r="AP42" s="49"/>
-      <c r="AQ42" s="28"/>
-      <c r="AR42" s="28"/>
-      <c r="AS42" s="28"/>
-      <c r="AT42" s="28"/>
-      <c r="AU42" s="28"/>
-      <c r="AV42" s="49"/>
-      <c r="AW42" s="28"/>
-      <c r="AX42" s="28"/>
-      <c r="AY42" s="28"/>
-      <c r="AZ42" s="43"/>
+        <v>79</v>
+      </c>
+      <c r="B42" s="32"/>
+      <c r="C42" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="48"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AI42" s="2"/>
+      <c r="AJ42" s="48"/>
+      <c r="AK42" s="2"/>
+      <c r="AL42" s="2"/>
+      <c r="AM42" s="2"/>
+      <c r="AN42" s="51"/>
+      <c r="AO42" s="2"/>
+      <c r="AP42" s="48"/>
+      <c r="AQ42" s="2"/>
+      <c r="AR42" s="2"/>
+      <c r="AS42" s="2"/>
+      <c r="AT42" s="2"/>
+      <c r="AU42" s="2"/>
+      <c r="AV42" s="48"/>
+      <c r="AW42" s="2"/>
+      <c r="AX42" s="2"/>
+      <c r="AY42" s="2"/>
+      <c r="AZ42" s="44"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AA43" s="3"/>
-      <c r="AB43" s="3"/>
-      <c r="AC43" s="3"/>
-      <c r="AD43" s="49"/>
-      <c r="AE43" s="3"/>
-      <c r="AF43" s="3"/>
-      <c r="AG43" s="3"/>
-      <c r="AH43" s="3"/>
-      <c r="AI43" s="3"/>
-      <c r="AJ43" s="49"/>
-      <c r="AK43" s="3"/>
-      <c r="AL43" s="3"/>
-      <c r="AM43" s="3"/>
-      <c r="AN43" s="3"/>
-      <c r="AO43" s="3"/>
-      <c r="AP43" s="49"/>
-      <c r="AQ43" s="3"/>
-      <c r="AR43" s="3"/>
-      <c r="AS43" s="3"/>
-      <c r="AT43" s="3"/>
-      <c r="AU43" s="3"/>
-      <c r="AV43" s="49"/>
-      <c r="AW43" s="3"/>
-      <c r="AX43" s="3"/>
-      <c r="AY43" s="3"/>
-      <c r="AZ43" s="43"/>
+        <v>79</v>
+      </c>
+      <c r="B43" s="32"/>
+      <c r="C43" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="48"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="2"/>
+      <c r="AI43" s="2"/>
+      <c r="AJ43" s="48"/>
+      <c r="AK43" s="2"/>
+      <c r="AL43" s="2"/>
+      <c r="AM43" s="2"/>
+      <c r="AN43" s="51"/>
+      <c r="AO43" s="2"/>
+      <c r="AP43" s="48"/>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="2"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="48"/>
+      <c r="AW43" s="2"/>
+      <c r="AX43" s="2"/>
+      <c r="AY43" s="2"/>
+      <c r="AZ43" s="44"/>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="3"/>
-      <c r="AC44" s="3"/>
-      <c r="AD44" s="49"/>
-      <c r="AE44" s="3"/>
-      <c r="AF44" s="3"/>
-      <c r="AG44" s="3"/>
-      <c r="AH44" s="3"/>
-      <c r="AI44" s="3"/>
-      <c r="AJ44" s="49"/>
-      <c r="AK44" s="3"/>
-      <c r="AL44" s="3"/>
-      <c r="AM44" s="3"/>
-      <c r="AN44" s="3"/>
-      <c r="AO44" s="3"/>
-      <c r="AP44" s="49"/>
-      <c r="AQ44" s="3"/>
-      <c r="AR44" s="3"/>
-      <c r="AS44" s="3"/>
-      <c r="AT44" s="3"/>
-      <c r="AU44" s="3"/>
-      <c r="AV44" s="49"/>
-      <c r="AW44" s="3"/>
-      <c r="AX44" s="3"/>
-      <c r="AY44" s="3"/>
-      <c r="AZ44" s="43"/>
+        <v>87</v>
+      </c>
+      <c r="B44" s="34"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="P44" s="28"/>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="28"/>
+      <c r="U44" s="28"/>
+      <c r="V44" s="28"/>
+      <c r="W44" s="28"/>
+      <c r="X44" s="28"/>
+      <c r="Y44" s="28"/>
+      <c r="Z44" s="28"/>
+      <c r="AA44" s="28"/>
+      <c r="AB44" s="28"/>
+      <c r="AC44" s="28"/>
+      <c r="AD44" s="48"/>
+      <c r="AE44" s="28"/>
+      <c r="AF44" s="28"/>
+      <c r="AG44" s="28"/>
+      <c r="AH44" s="28"/>
+      <c r="AI44" s="28"/>
+      <c r="AJ44" s="48"/>
+      <c r="AK44" s="28"/>
+      <c r="AL44" s="28"/>
+      <c r="AM44" s="28"/>
+      <c r="AN44" s="28"/>
+      <c r="AO44" s="28"/>
+      <c r="AP44" s="48"/>
+      <c r="AQ44" s="28"/>
+      <c r="AR44" s="28"/>
+      <c r="AS44" s="28"/>
+      <c r="AT44" s="28"/>
+      <c r="AU44" s="28"/>
+      <c r="AV44" s="48"/>
+      <c r="AW44" s="28"/>
+      <c r="AX44" s="28"/>
+      <c r="AY44" s="28"/>
+      <c r="AZ44" s="44"/>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35" t="s">
+        <v>3</v>
+      </c>
       <c r="C45" s="10"/>
       <c r="D45" s="13"/>
       <c r="E45" s="5"/>
@@ -3829,37 +3795,35 @@
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
-      <c r="AD45" s="49"/>
+      <c r="AD45" s="48"/>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
-      <c r="AJ45" s="49"/>
+      <c r="AJ45" s="48"/>
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
       <c r="AN45" s="3"/>
-      <c r="AO45" s="3"/>
-      <c r="AP45" s="49"/>
-      <c r="AQ45" s="3"/>
-      <c r="AR45" s="3"/>
-      <c r="AS45" s="3"/>
-      <c r="AT45" s="3"/>
-      <c r="AU45" s="3"/>
-      <c r="AV45" s="49"/>
-      <c r="AW45" s="3"/>
-      <c r="AX45" s="3"/>
-      <c r="AY45" s="3"/>
-      <c r="AZ45" s="43"/>
+      <c r="AO45" s="51"/>
+      <c r="AP45" s="48"/>
+      <c r="AQ45" s="51"/>
+      <c r="AR45" s="51"/>
+      <c r="AS45" s="51"/>
+      <c r="AT45" s="51"/>
+      <c r="AU45" s="51"/>
+      <c r="AV45" s="48"/>
+      <c r="AW45" s="51"/>
+      <c r="AX45" s="51"/>
+      <c r="AY45" s="51"/>
+      <c r="AZ45" s="44"/>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>55</v>
-      </c>
+      <c r="B46" s="35"/>
       <c r="C46" s="10"/>
       <c r="D46" s="13"/>
       <c r="E46" s="5"/>
@@ -3887,35 +3851,35 @@
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
-      <c r="AD46" s="49"/>
+      <c r="AD46" s="48"/>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
-      <c r="AJ46" s="49"/>
+      <c r="AJ46" s="48"/>
       <c r="AK46" s="3"/>
       <c r="AL46" s="3"/>
       <c r="AM46" s="3"/>
       <c r="AN46" s="3"/>
       <c r="AO46" s="3"/>
-      <c r="AP46" s="49"/>
+      <c r="AP46" s="48"/>
       <c r="AQ46" s="3"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
       <c r="AT46" s="3"/>
       <c r="AU46" s="3"/>
-      <c r="AV46" s="49"/>
+      <c r="AV46" s="48"/>
       <c r="AW46" s="3"/>
       <c r="AX46" s="3"/>
       <c r="AY46" s="3"/>
-      <c r="AZ46" s="43"/>
+      <c r="AZ46" s="44"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="32"/>
+      <c r="B47" s="36"/>
       <c r="C47" s="10"/>
       <c r="D47" s="13"/>
       <c r="E47" s="5"/>
@@ -3943,35 +3907,37 @@
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
-      <c r="AD47" s="49"/>
+      <c r="AD47" s="48"/>
       <c r="AE47" s="3"/>
       <c r="AF47" s="3"/>
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
-      <c r="AJ47" s="49"/>
+      <c r="AJ47" s="48"/>
       <c r="AK47" s="3"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="3"/>
       <c r="AN47" s="3"/>
       <c r="AO47" s="3"/>
-      <c r="AP47" s="49"/>
+      <c r="AP47" s="48"/>
       <c r="AQ47" s="3"/>
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
       <c r="AU47" s="3"/>
-      <c r="AV47" s="49"/>
+      <c r="AV47" s="48"/>
       <c r="AW47" s="3"/>
       <c r="AX47" s="3"/>
       <c r="AY47" s="3"/>
-      <c r="AZ47" s="43"/>
+      <c r="AZ47" s="44"/>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="35"/>
+      <c r="B48" s="32" t="s">
+        <v>55</v>
+      </c>
       <c r="C48" s="10"/>
       <c r="D48" s="13"/>
       <c r="E48" s="5"/>
@@ -3999,39 +3965,37 @@
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="3"/>
-      <c r="AD48" s="49"/>
+      <c r="AD48" s="48"/>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
-      <c r="AJ48" s="49"/>
+      <c r="AJ48" s="48"/>
       <c r="AK48" s="3"/>
       <c r="AL48" s="3"/>
       <c r="AM48" s="3"/>
       <c r="AN48" s="3"/>
       <c r="AO48" s="3"/>
-      <c r="AP48" s="49"/>
-      <c r="AQ48" s="3"/>
-      <c r="AR48" s="3"/>
-      <c r="AS48" s="3"/>
-      <c r="AT48" s="3"/>
-      <c r="AU48" s="3"/>
-      <c r="AV48" s="49"/>
-      <c r="AW48" s="3"/>
-      <c r="AX48" s="3"/>
-      <c r="AY48" s="3"/>
-      <c r="AZ48" s="43"/>
-    </row>
-    <row r="49" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="41" t="s">
+      <c r="AP48" s="48"/>
+      <c r="AQ48" s="51"/>
+      <c r="AR48" s="51"/>
+      <c r="AS48" s="51"/>
+      <c r="AT48" s="51"/>
+      <c r="AU48" s="51"/>
+      <c r="AV48" s="48"/>
+      <c r="AW48" s="51"/>
+      <c r="AX48" s="51"/>
+      <c r="AY48" s="51"/>
+      <c r="AZ48" s="44"/>
+    </row>
+    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A49" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="16"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="13"/>
       <c r="E49" s="5"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -4057,34 +4021,152 @@
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
-      <c r="AD49" s="49"/>
+      <c r="AD49" s="48"/>
       <c r="AE49" s="3"/>
       <c r="AF49" s="3"/>
       <c r="AG49" s="3"/>
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
-      <c r="AJ49" s="49"/>
+      <c r="AJ49" s="48"/>
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="3"/>
       <c r="AN49" s="3"/>
       <c r="AO49" s="3"/>
-      <c r="AP49" s="49"/>
+      <c r="AP49" s="48"/>
       <c r="AQ49" s="3"/>
       <c r="AR49" s="3"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="3"/>
       <c r="AU49" s="3"/>
-      <c r="AV49" s="49"/>
+      <c r="AV49" s="48"/>
       <c r="AW49" s="3"/>
       <c r="AX49" s="3"/>
       <c r="AY49" s="3"/>
       <c r="AZ49" s="44"/>
     </row>
-    <row r="50" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A50" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="35"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3"/>
+      <c r="AC50" s="3"/>
+      <c r="AD50" s="48"/>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="3"/>
+      <c r="AG50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="48"/>
+      <c r="AK50" s="3"/>
+      <c r="AL50" s="3"/>
+      <c r="AM50" s="3"/>
+      <c r="AN50" s="3"/>
+      <c r="AO50" s="3"/>
+      <c r="AP50" s="48"/>
+      <c r="AQ50" s="3"/>
+      <c r="AR50" s="3"/>
+      <c r="AS50" s="3"/>
+      <c r="AT50" s="3"/>
+      <c r="AU50" s="3"/>
+      <c r="AV50" s="48"/>
+      <c r="AW50" s="3"/>
+      <c r="AX50" s="3"/>
+      <c r="AY50" s="3"/>
+      <c r="AZ50" s="44"/>
+    </row>
+    <row r="51" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="46"/>
+      <c r="AE51" s="3"/>
+      <c r="AF51" s="3"/>
+      <c r="AG51" s="3"/>
+      <c r="AH51" s="3"/>
+      <c r="AI51" s="3"/>
+      <c r="AJ51" s="46"/>
+      <c r="AK51" s="3"/>
+      <c r="AL51" s="3"/>
+      <c r="AM51" s="3"/>
+      <c r="AN51" s="3"/>
+      <c r="AO51" s="3"/>
+      <c r="AP51" s="46"/>
+      <c r="AQ51" s="51"/>
+      <c r="AR51" s="51"/>
+      <c r="AS51" s="51"/>
+      <c r="AT51" s="51"/>
+      <c r="AU51" s="51"/>
+      <c r="AV51" s="46"/>
+      <c r="AW51" s="51"/>
+      <c r="AX51" s="51"/>
+      <c r="AY51" s="51"/>
+      <c r="AZ51" s="45"/>
+    </row>
+    <row r="52" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="AZ2:AZ49"/>
+  <mergeCells count="5">
+    <mergeCell ref="AD4:AD51"/>
+    <mergeCell ref="AJ4:AJ51"/>
+    <mergeCell ref="AP4:AP51"/>
+    <mergeCell ref="AV4:AV51"/>
+    <mergeCell ref="AZ4:AZ51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>